<commit_message>
latest batch of data
</commit_message>
<xml_diff>
--- a/allegro/PJH F41225 - BOM gps_interface_boardv51ph_smoothed_BOM-AlternativePartNumberRequestReport.xlsx
+++ b/allegro/PJH F41225 - BOM gps_interface_boardv51ph_smoothed_BOM-AlternativePartNumberRequestReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ppfs6.physics.ox.ac.uk\CEG\Central Electronics\Projects\Hastingsp\DUNE\upenn-dune-gib\allegro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A143B86C-47B4-43CC-87AF-4D80BFBE5BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF12CE9-E847-4931-8811-D7019C2CF1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="375" windowWidth="30675" windowHeight="17250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="5100" windowWidth="33180" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>MAX9371EKA+</t>
   </si>
   <si>
-    <t>Please an alternative as this is not available with suppliers</t>
-  </si>
-  <si>
     <t>J1,J4,J5,J6</t>
   </si>
   <si>
@@ -190,14 +187,17 @@
     <t>Farnell 3471205</t>
   </si>
   <si>
-    <t>Seems only available in SOIC8 - needs a change our end or left off build</t>
+    <t>I have sent updated design data that uses the SOIC variant listed to the left.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX9371ESA+ </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -235,6 +235,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -295,7 +311,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -317,6 +333,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -626,7 +648,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +794,7 @@
         <v>30</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>31</v>
@@ -795,7 +817,7 @@
         <v>36</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>37</v>
@@ -818,7 +840,7 @@
         <v>39</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>40</v>
@@ -837,37 +859,37 @@
       <c r="D26" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="11" t="s">
         <v>56</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="10" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="D27" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="E27" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="F27" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -881,5 +903,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>